<commit_message>
bahan setengah jadi done
</commit_message>
<xml_diff>
--- a/upload/template-raw-materals.xlsx
+++ b/upload/template-raw-materals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB04B80C-BB3C-2D43-A422-FF256C77E3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0DFC5C-1BEF-E946-ADF0-3CD302990733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="500" windowWidth="22660" windowHeight="14260" xr2:uid="{7518A780-8C7C-49F0-AF96-CB417392CB7C}"/>
   </bookViews>
@@ -59,10 +59,10 @@
     <t>Raw Material</t>
   </si>
   <si>
-    <t>gr</t>
-  </si>
-  <si>
-    <t>Tepung Terigu</t>
+    <t>Telur</t>
+  </si>
+  <si>
+    <t>pcs</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -469,23 +469,23 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44998</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>44993</v>
-      </c>
-      <c r="C2">
-        <v>10000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2">
-        <v>300000</v>
+        <v>18000</v>
       </c>
       <c r="F2">
         <f>E2/C2</f>
-        <v>30</v>
+        <v>1125</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>

</xml_diff>